<commit_message>
COMMIT_DL_DOMICILE après ajout dans questions_a_traiter
</commit_message>
<xml_diff>
--- a/questions_a_traiter/Questions_a_traiter.xlsx
+++ b/questions_a_traiter/Questions_a_traiter.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>PMD</t>
   </si>
@@ -136,7 +136,8 @@
     <t xml:space="preserve">Exporter ou importer : \Workspace\.metadata\.plugins\net.sourceforge.pmd.eclipse.plugin\ruleset.xml </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;plugin&gt;
+    <t xml:space="preserve">
+&lt;plugin&gt;
    &lt;groupId&gt;org.apache.maven.plugins&lt;/groupId&gt;
    &lt;artifactId&gt;maven-compiler-plugin&lt;/artifactId&gt;
    &lt;configuration&gt;
@@ -145,6 +146,34 @@
    &lt;/configuration&gt;
 &lt;/plugin&gt; 
 </t>
+  </si>
+  <si>
+    <t>Choix du HTML</t>
+  </si>
+  <si>
+    <t>Faut-il choisir HTML5 ou XHTML1.0 Transitional dans les jsp ?</t>
+  </si>
+  <si>
+    <t>Log4j2.xml</t>
+  </si>
+  <si>
+    <t>A quoi sert et comment utiliser le Log4j2.xml ?</t>
+  </si>
+  <si>
+    <t>Apparemment, Tomcat utilise un Log4j2.xml. Pourquoi ? (pas un simple Log4j.properties),
+Pourrais-je voir un exemple de Log4j2.xml bien implémenté ?</t>
+  </si>
+  <si>
+    <t>Test d'un controller Servlet</t>
+  </si>
+  <si>
+    <t>Comment implémenter une org.apache….Request (héritant de HttpServletRequest) pour tester une méthode doGet(….) d'un controller Servlet ?</t>
+  </si>
+  <si>
+    <t>Il pourrait être intéressant de tester un controller Servlet sans lancer l'appli web et donc Tomcat. Or, le conteneur de Servlet Tomcat fournit les HttpServletRequest et HttpServletResponse à passer aux méthodes doHead, doGet et doPost du controller Servlet. Comment instancier une HttpServletRequest dans un test unitaire JUnit en lui passant des paramètres ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACAI préconise l'utilisation de </t>
   </si>
 </sst>
 </file>
@@ -553,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E22"/>
+  <dimension ref="B2:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -597,7 +626,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" ht="127.5" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
@@ -611,88 +640,106 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
+    <row r="7" spans="2:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+    <row r="8" spans="2:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="2:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="2:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5"/>
+    <row r="11" spans="2:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
+    <row r="12" spans="2:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
@@ -752,10 +799,16 @@
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
COMMIT_DL_DOMICILE après question fil d'ariane
</commit_message>
<xml_diff>
--- a/questions_a_traiter/Questions_a_traiter.xlsx
+++ b/questions_a_traiter/Questions_a_traiter.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>PMD</t>
   </si>
@@ -174,6 +174,16 @@
   </si>
   <si>
     <t xml:space="preserve">ACAI préconise l'utilisation de </t>
+  </si>
+  <si>
+    <t>Fil d'ariane</t>
+  </si>
+  <si>
+    <t>Comment implémenter un fil d'ariane dans l'application (breadcrumbs) ?</t>
+  </si>
+  <si>
+    <t>Un fil d'ariane est utile pour l'utilisateur en haut de chaque jsp.
+Comment implémenter ce fil d'ariane avec Springweb mvc ?</t>
   </si>
 </sst>
 </file>
@@ -584,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -742,10 +752,16 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5"/>
+    <row r="13" spans="2:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
COMMIT_DL_DOMICILE après questions à traiter
</commit_message>
<xml_diff>
--- a/questions_a_traiter/Questions_a_traiter.xlsx
+++ b/questions_a_traiter/Questions_a_traiter.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Donnees\eclipse\eclipseworkspace_neon\traficweb_maven\questions_a_traiter\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14100" windowHeight="10095"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14100" windowHeight="10095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>PMD</t>
-  </si>
-  <si>
-    <t>Description</t>
   </si>
   <si>
     <t>Comment s'échanger les règles de PMD ?</t>
@@ -178,9 +181,6 @@
 Possibilité de loger directement dans le bdd par config.(apender)</t>
   </si>
   <si>
-    <t>Donc pas de spring boot, l'utilité est restreinte et la génération du war peut gêner des incompatibilités avec le tomvat de prod.</t>
-  </si>
-  <si>
     <t>Fil d'Ariane</t>
   </si>
   <si>
@@ -195,13 +195,90 @@
   </si>
   <si>
     <t xml:space="preserve">Test intégré avec Selenium ou test unitaire avec mokito </t>
+  </si>
+  <si>
+    <t>Remarques</t>
+  </si>
+  <si>
+    <t>KO - NE FONCTIONNE PAS.
+Cf mon mail du 04/09/2017 à 10h31</t>
+  </si>
+  <si>
+    <t>Donc pas de spring boot, l'utilité est restreinte et la génération du war peut gêner des incompatibilités avec le tomcat de prod.</t>
+  </si>
+  <si>
+    <t>Je croyais que nous avions décider de regarder si il était possible de :
+- Utiliser quand même SpringBoot pour le cas où l'on voudrait fournir des distributions complètes (avec Tomcat embarqué),
+- Voir si on pouvait paramétrer SpringBoot de sorte à pouvoir sortir Tomcat du livrable si le centre serveur le souhaitait.
+Ainsi, nous couvrions tous les cas de figure.</t>
+  </si>
+  <si>
+    <t>KO - NE FONCTIONNE PAS.
+J'ai exporté le ruleset.xml depuis \Workspace\.metadata\.plugins\net.sourceforge.pmd.eclipse.plugin\ruleset.xml sur ma machine et l'ai copié au même endroit dans un même Eclipse Neon 3 sur une autre machine.
+Je n'ai pas récupéré les règles et leur état d'activation après avoir fait "importer un nouvel ensemble de règles".
+Cf mon mail du 06/09/2017 12:18</t>
+  </si>
+  <si>
+    <t>Extrêmement intéressant. A CREUSER.</t>
+  </si>
+  <si>
+    <t>J'ai besoin de plus d'explications. Quand faut-il fournir un Log4j2.xml ? A CREUSER.</t>
+  </si>
+  <si>
+    <t>Eclipse</t>
+  </si>
+  <si>
+    <t>Comment bien paramétrer les projets Eclipse afin d'en simplifier l'échange ?</t>
+  </si>
+  <si>
+    <t>On rencontre de nombreux problèmes lors de l'échange de projets Eclipse :
+- Encodage des messages dans la console défectueux.
+- Paramétrage compliqué du projet chez le destinataire avant de pouvoir faire fonctionner le projet.
+Comment bien paramétrer les projets pour simplifier l'installation du projet chez le destinataire ?</t>
+  </si>
+  <si>
+    <t>Description de la question</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Fixer l'encodage du projet </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Click droit projet &gt; Propriétés &gt; Resources &gt; Text File Encoding : other ----&gt; UTF-8 et New Text File Line Delimiter : other -----&gt; Windows
+A POURSUIVRE</t>
+    </r>
+  </si>
+  <si>
+    <t>servlet-api</t>
+  </si>
+  <si>
+    <t>Quelle stratégie adopter concernant servlet-api.jar dans les projets web Eclipse ?</t>
+  </si>
+  <si>
+    <t>Un projet web avec Servlets a besoin de servlet-api.jar pour fonctionner. Or, le conteneur de Servlet (Tomcat) fournit ce jar.
+Du coup, si on ne fournit pas la librairie servlet-api.jar dans un projet Eclipse, le destinataire verra des erreurs dans son projet Eclipse tant qu'il n'y aura pas importé les librairies de Tomcat.
+Inversement, si on fournit cette librairie et que l'on s'appuie sur la librairie fournie pour écrire les Servlets, quelle sera la librairie servlet-api.jar réellement utilisée lors du déploiement en centre serveur ? Celle du Tomcat du centre serveur ? La librairie fournie ?
+Quelle stratégie adopter concernant servlet-api.jar ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -227,8 +304,34 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +341,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -292,10 +407,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -604,18 +734,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -624,237 +754,299 @@
     <col min="2" max="2" width="27.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="41.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="103" style="1" customWidth="1"/>
-    <col min="5" max="5" width="80.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="5" max="6" width="80.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" s="3" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="117" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="2:6" ht="127.5" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" ht="127.5" x14ac:dyDescent="0.2">
-      <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="F5" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="2:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="2:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="C10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="2:6" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="2:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="C12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="9" t="s">
+      <c r="F12" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="2:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>